<commit_message>
Updated definition processor assets to support FixedLists's DisplayOrder
</commit_message>
<xml_diff>
--- a/src/test/fixtures/sheet/definition.xlsx
+++ b/src/test/fixtures/sheet/definition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markry/workspace/hmcts/ccd-definition-processor/src/test/fixtures/sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesne@kainos.com/Documents/HMCTS/ccd-definition-processor/src/test/fixtures/sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4AFDBB-2518-1B4A-AE55-15474673A915}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC27219-731C-6D47-AF58-B0F613A855E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1940" windowWidth="27640" windowHeight="13980" tabRatio="500" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="1940" windowWidth="27640" windowHeight="13980" tabRatio="500" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="178">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>Numbered order of fixed list items</t>
   </si>
 </sst>
 </file>
@@ -1465,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1477,7 +1480,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>126</v>
       </c>
@@ -1492,7 +1495,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1508,8 +1511,11 @@
       <c r="E2" s="13" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1524,6 +1530,9 @@
       </c>
       <c r="E3" s="9" t="s">
         <v>130</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E924DBEA-AE14-AF45-AB43-4428B6C060F3}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Shuttered column for xls/json gen on Jurisdiction
</commit_message>
<xml_diff>
--- a/src/test/fixtures/sheet/definition.xlsx
+++ b/src/test/fixtures/sheet/definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="185">
   <si>
     <t xml:space="preserve">Jurisdiction</t>
   </si>
@@ -87,10 +87,16 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Shuttered</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">CaseRoles</t>
@@ -915,7 +921,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -961,6 +967,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1234,10 +1244,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="P2:Q3 E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1278,7 +1288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1293,6 +1303,9 @@
       </c>
       <c r="E3" s="10" t="s">
         <v>13</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1306,10 +1319,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1331,7 +1347,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="P2:Q3 F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1342,7 +1358,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1362,17 +1378,17 @@
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>139</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1386,13 +1402,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1430,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1425,7 +1441,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1453,38 +1469,38 @@
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>144</v>
       </c>
+      <c r="D2" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>146</v>
+      </c>
       <c r="H2" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>26</v>
+        <v>147</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1494,38 +1510,38 @@
       <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="43" t="s">
-        <v>98</v>
+      <c r="D3" s="44" t="s">
+        <v>100</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="K3" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1547,7 +1563,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1558,19 +1574,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -1580,16 +1596,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,17 +1615,17 @@
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>62</v>
+      <c r="C3" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1631,7 +1647,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1642,7 +1658,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1664,16 +1680,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,17 +1699,17 @@
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>62</v>
+      <c r="C3" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1715,7 +1731,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="P2:Q3 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1728,41 +1744,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="48"/>
+      <c r="A3" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="49"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
@@ -1785,7 +1801,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1796,7 +1812,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1818,16 +1834,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,17 +1853,17 @@
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>62</v>
+      <c r="C3" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1869,7 +1885,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1879,20 +1895,20 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="49" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="50" t="s">
+      <c r="A1" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -1902,16 +1918,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,17 +1937,17 @@
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>62</v>
+      <c r="C3" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1953,7 +1969,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1964,7 +1980,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1987,13 +2003,13 @@
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,16 +2020,16 @@
         <v>10</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="D3" s="21" t="s">
         <v>169</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2035,7 +2051,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2046,7 +2062,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2067,13 +2083,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2083,14 +2099,14 @@
       <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>63</v>
+      <c r="C3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2112,7 +2128,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2122,8 +2138,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="53" t="s">
-        <v>175</v>
+      <c r="A1" s="54" t="s">
+        <v>177</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2134,8 +2150,8 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
     </row>
     <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -2145,36 +2161,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>176</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2196,7 +2212,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="P2:Q3 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2208,10 +2224,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -2222,17 +2238,17 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>18</v>
+      <c r="A2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,10 +2258,10 @@
       <c r="B3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -2274,7 +2290,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2285,7 +2301,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2307,16 +2323,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2326,17 +2342,17 @@
       <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>63</v>
+      <c r="C3" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>65</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2358,7 +2374,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2369,15 +2385,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6"/>
@@ -2391,16 +2407,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="59" t="s">
-        <v>181</v>
+        <v>178</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>183</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,17 +2426,17 @@
       <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>63</v>
+      <c r="C3" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>65</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2442,7 +2458,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2452,8 +2468,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>20</v>
+      <c r="A1" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2480,52 +2496,52 @@
       <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>24</v>
       </c>
+      <c r="F2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="H2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="43" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>30</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2547,7 +2563,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2558,7 +2574,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2586,34 +2602,34 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>26</v>
+      <c r="H2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2623,35 +2639,35 @@
       <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>19</v>
+      <c r="C3" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +2689,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="P2:Q3 I4"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2684,7 +2700,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="3" t="s">
@@ -2712,34 +2728,34 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="F2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="G2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="H2" s="24" t="s">
         <v>55</v>
       </c>
+      <c r="I2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>57</v>
+      </c>
       <c r="K2" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2749,35 +2765,35 @@
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>19</v>
+      <c r="C3" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="15" t="s">
         <v>63</v>
       </c>
+      <c r="H3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>65</v>
+      </c>
       <c r="J3" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2798,8 +2814,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2:Q3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2810,7 +2826,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2841,49 +2857,49 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,50 +2909,50 @@
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>62</v>
+      <c r="C3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>88</v>
+        <v>67</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>90</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2958,121 +2974,121 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="P2:Q3 D6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="26" width="30.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="26" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="26" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="26" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="26" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="26" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="14" style="27" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="28" width="6.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="27" width="30.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="27" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="27" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="27" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="27" width="6.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="14" style="28" width="6.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="29" width="6.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="37" customFormat="true" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+    <row r="2" s="38" customFormat="true" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="35" t="s">
+      <c r="C2" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="D2" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-    </row>
-    <row r="3" s="27" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
+      <c r="G2" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+    </row>
+    <row r="3" s="28" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="40" t="s">
+      <c r="D3" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="G3" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>65</v>
+      <c r="H3" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3094,7 +3110,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3105,7 +3121,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3129,22 +3145,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3154,8 +3170,8 @@
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>19</v>
+      <c r="C3" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>11</v>
@@ -3167,10 +3183,10 @@
         <v>13</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3192,7 +3208,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P2:Q3 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3203,7 +3219,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3219,12 +3235,12 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -3239,58 +3255,58 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>26</v>
+        <v>119</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3300,8 +3316,8 @@
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>19</v>
+      <c r="C3" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>11</v>
@@ -3313,46 +3329,46 @@
         <v>13</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="J3" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="I3" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="J3" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="K3" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="L3" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="M3" s="43" t="s">
         <v>130</v>
       </c>
+      <c r="N3" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="O3" s="43" t="s">
+        <v>132</v>
+      </c>
       <c r="P3" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="S3" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="R3" s="20" t="s">
         <v>134</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>